<commit_message>
completed MVC for donor file checker.
</commit_message>
<xml_diff>
--- a/src/main/java/corecentra/qaqctool/storage/task_test.xlsx
+++ b/src/main/java/corecentra/qaqctool/storage/task_test.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS\3_Spring2022\5500\old project\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D879CD99-8336-4BD4-AD96-15290091D84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1083A2DB-A110-42C4-9EE4-5504A7B05FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{D4DDA300-9C13-4F0E-9DF5-732A48B3DFD5}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{D45B6B4B-F0F5-45B4-9097-F89309CE0147}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tasks" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,96 +35,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
-  <si>
-    <t>Project ID
-varchar(8)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t>Lock</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Food and Water</t>
+  </si>
+  <si>
+    <t>06/05/2019</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Main City</t>
+  </si>
+  <si>
+    <t>Gallons of water distributed</t>
+  </si>
+  <si>
+    <t>RS0001</t>
+  </si>
+  <si>
+    <t>PRJ0001</t>
+  </si>
+  <si>
+    <t>Delete Locked</t>
+  </si>
+  <si>
+    <t>Scorecard Report</t>
+  </si>
+  <si>
+    <t>Impact Indicator</t>
+  </si>
+  <si>
+    <t>Date Created
+varchar(45)</t>
+  </si>
+  <si>
+    <t>Reporting Year
+varchar(45)</t>
+  </si>
+  <si>
+    <t>Results Yield (#)
+decimal(16,2)</t>
+  </si>
+  <si>
+    <t>Region/Area
+varchar(100)</t>
+  </si>
+  <si>
+    <t>Result
+varchar(100)</t>
+  </si>
+  <si>
+    <t>Result ID
+varchar(100)</t>
   </si>
   <si>
     <t>Project Name
 varchar(128)</t>
   </si>
   <si>
-    <t>Task ID
-Int Auto Increment</t>
-  </si>
-  <si>
-    <t>Task
-varchar(96)</t>
-  </si>
-  <si>
-    <t>Percent Complete
-int</t>
-  </si>
-  <si>
-    <t>Owner
-varchar(24)</t>
-  </si>
-  <si>
-    <t>Start Date
-varchar(45)</t>
-  </si>
-  <si>
-    <t>End Date
-varchar(45)</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Flag</t>
-  </si>
-  <si>
-    <t>Original End Date</t>
-  </si>
-  <si>
-    <t>Progress Flag</t>
-  </si>
-  <si>
-    <t>Delete Locked</t>
-  </si>
-  <si>
-    <t>Details</t>
-  </si>
-  <si>
-    <t>PRJ0001</t>
-  </si>
-  <si>
-    <t>Clean Water Distribution</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Contact Jeff at Clean Water Inc for pricing</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>Jim</t>
-  </si>
-  <si>
-    <t>06/14/2019</t>
-  </si>
-  <si>
-    <t>01/14/2020</t>
-  </si>
-  <si>
-    <t>On Track</t>
-  </si>
-  <si>
-    <t>GREEN</t>
-  </si>
-  <si>
-    <t>Lock</t>
+    <t>Project ID
+varchar(50)</t>
+  </si>
+  <si>
+    <t>2a14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -143,6 +131,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -186,12 +181,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -507,22 +509,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E11425EA-3545-4A54-B9EA-5EB5F50F08A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04E04E4-BE78-4586-A8B1-AC531432E9DF}">
   <sheetPr>
     <tabColor rgb="FF2E75B5"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.40625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="8.86328125" customWidth="1"/>
+    <col min="1" max="1" width="16.6796875" customWidth="1"/>
     <col min="2" max="3" width="20.26953125" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
+    <col min="4" max="4" width="25.1328125" customWidth="1"/>
     <col min="5" max="5" width="20.26953125" customWidth="1"/>
     <col min="6" max="6" width="13.26953125" customWidth="1"/>
     <col min="7" max="7" width="14.6796875" customWidth="1"/>
@@ -532,100 +534,340 @@
     <col min="11" max="11" width="13.40625" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
     <col min="13" max="13" width="24.6796875" customWidth="1"/>
-    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="14" max="26" width="8.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="44.25" x14ac:dyDescent="0.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" ht="39.75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="14.75" x14ac:dyDescent="0.75">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="29.5" x14ac:dyDescent="0.75">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B755AE6C24C73342B92942696AC765F8" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a7176e845c84254584adff52c69aa50e">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="467e4c5d-19c7-4b8f-8b29-7da05b79a901" xmlns:ns4="7a23d9ff-ea04-4caf-be8d-fe992a91c2c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9de1e32bb1ce28059a55427a752b2c92" ns3:_="" ns4:_="">
+    <xsd:import namespace="467e4c5d-19c7-4b8f-8b29-7da05b79a901"/>
+    <xsd:import namespace="7a23d9ff-ea04-4caf-be8d-fe992a91c2c1"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceFastMetadata" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="467e4c5d-19c7-4b8f-8b29-7da05b79a901" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="10" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7a23d9ff-ea04-4caf-be8d-fe992a91c2c1" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7533D79D-A843-4455-BDF2-0E10894BB96A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="467e4c5d-19c7-4b8f-8b29-7da05b79a901"/>
+    <ds:schemaRef ds:uri="7a23d9ff-ea04-4caf-be8d-fe992a91c2c1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87252CEF-0036-4AB4-8075-E190D9A87764}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7a23d9ff-ea04-4caf-be8d-fe992a91c2c1"/>
+    <ds:schemaRef ds:uri="467e4c5d-19c7-4b8f-8b29-7da05b79a901"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D649B71C-9962-4406-AA88-1E55CB4BDF6B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>